<commit_message>
sql with dummy data and txt with passwords
</commit_message>
<xml_diff>
--- a/toy info for database.xlsx
+++ b/toy info for database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ASE230-F22-FooCy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04211FC-C4EF-4352-BEE7-762BF26F54EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DC7F01-B800-4E0F-8958-CBB088529743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{52347841-8C47-4D3B-9938-8A4F7D54BC8C}"/>
+    <workbookView xWindow="30888" yWindow="12516" windowWidth="11844" windowHeight="7572" activeTab="2" xr2:uid="{52347841-8C47-4D3B-9938-8A4F7D54BC8C}"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
   <si>
     <t>Your pet's name engraved on a hand-painted woodcut ornament</t>
   </si>
@@ -296,6 +296,15 @@
   </si>
   <si>
     <t>Pet Supplies</t>
+  </si>
+  <si>
+    <t>seller01</t>
+  </si>
+  <si>
+    <t>seller02</t>
+  </si>
+  <si>
+    <t>admin3</t>
   </si>
 </sst>
 </file>
@@ -1260,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9A8051-5724-4E2E-B27C-EA626CB35747}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -1340,15 +1349,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326E6627-C5F3-4A03-9E83-CFC22186447F}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1364,26 +1377,26 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1399,12 +1412,12 @@
       <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>123456</v>
+      </c>
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
       <c r="H2" t="s">
         <v>20</v>
       </c>
@@ -1412,13 +1425,16 @@
         <v>20</v>
       </c>
       <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1434,12 +1450,12 @@
       <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>789456</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
       <c r="H3" t="s">
         <v>20</v>
       </c>
@@ -1447,13 +1463,16 @@
         <v>20</v>
       </c>
       <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1470,25 +1489,28 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
       <c r="H4" t="s">
         <v>20</v>
       </c>
       <c r="I4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1">
         <v>44903.164814814816</v>
       </c>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1505,25 +1527,28 @@
         <v>31</v>
       </c>
       <c r="F5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
       <c r="H5" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1">
         <v>44903.17355324074</v>
       </c>
-      <c r="K5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1540,21 +1565,24 @@
         <v>35</v>
       </c>
       <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
         <v>36</v>
       </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
       <c r="H6" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1">
         <v>44906.146782407406</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>